<commit_message>
Changed the code in app.py
Added comments in all files
</commit_message>
<xml_diff>
--- a/jupyter_files/New_AILandscape_allCompanies_100.xlsx
+++ b/jupyter_files/New_AILandscape_allCompanies_100.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sem 5\AI_Portfolio\jupyter_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B0F45E-B624-460C-AAC8-CB20CDE19D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265ACBEC-692F-4610-85D6-6B98A80C8B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="2004" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$101</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="383">
   <si>
     <t>Company</t>
   </si>
@@ -1172,12 +1172,6 @@
   </si>
   <si>
     <t>data lxtxr solutions production predictive cases analytics driven manufacturing complexity deploying intelligence integrating building products securing uvantage real maintenance external optimization reduce tier solution automotive time alternative sources lexatexer operations machine results provide case suppliers scheduling heavy machinery sales demand treasuries finance world integration legacy fraud industries corporates analysis focused onboarding problems process delivery analyze enterprise oee box language multiple mixed content failures automate understands integrate integrates reduces supplier quali powers power read types deliver reads type delivers generation japan singapore kudos german accelerator media life cycle management forecasts inventory detection retail smart factories learning honored partner make simplify creating operationalized achieve built software platforms managing analyzing solve broad range additional jump started needed cover entire drastically reducing secure fuse workbench automation covering suit supports inspection structured measurements unstructured reports</t>
-  </si>
-  <si>
-    <t>Manual Check</t>
-  </si>
-  <si>
-    <t>No mention of manufacturing industries</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1237,31 +1231,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1565,23 +1545,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1597,11 +1577,8 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>184</v>
       </c>
@@ -1620,11 +1597,8 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>38</v>
       </c>
@@ -1643,11 +1617,8 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>85</v>
       </c>
@@ -1666,11 +1637,8 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>60</v>
       </c>
@@ -1689,11 +1657,8 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>19</v>
       </c>
@@ -1712,11 +1677,8 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>173</v>
       </c>
@@ -1735,11 +1697,8 @@
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>94</v>
       </c>
@@ -1758,11 +1717,8 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>68</v>
       </c>
@@ -1775,11 +1731,8 @@
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>186</v>
       </c>
@@ -1798,11 +1751,8 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>212</v>
       </c>
@@ -1821,11 +1771,8 @@
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>107</v>
       </c>
@@ -1844,11 +1791,8 @@
       <c r="F12">
         <v>0</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>269</v>
       </c>
@@ -1867,11 +1811,8 @@
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>29</v>
       </c>
@@ -1884,11 +1825,8 @@
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>108</v>
       </c>
@@ -1907,11 +1845,8 @@
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>74</v>
       </c>
@@ -1924,11 +1859,8 @@
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>137</v>
       </c>
@@ -1947,11 +1879,8 @@
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>274</v>
       </c>
@@ -1970,11 +1899,8 @@
       <c r="F18">
         <v>0</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>209</v>
       </c>
@@ -1993,11 +1919,8 @@
       <c r="F19">
         <v>0</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>48</v>
       </c>
@@ -2016,11 +1939,8 @@
       <c r="F20">
         <v>0</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -2033,11 +1953,8 @@
       <c r="F21">
         <v>0</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>157</v>
       </c>
@@ -2056,11 +1973,8 @@
       <c r="F22">
         <v>0</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>13</v>
       </c>
@@ -2079,11 +1993,8 @@
       <c r="F23">
         <v>1</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>218</v>
       </c>
@@ -2102,11 +2013,8 @@
       <c r="F24">
         <v>1</v>
       </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>196</v>
       </c>
@@ -2119,14 +2027,8 @@
       <c r="F25">
         <v>0</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>201</v>
       </c>
@@ -2145,11 +2047,8 @@
       <c r="F26">
         <v>1</v>
       </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>203</v>
       </c>
@@ -2168,11 +2067,8 @@
       <c r="F27">
         <v>0</v>
       </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>200</v>
       </c>
@@ -2191,14 +2087,8 @@
       <c r="F28">
         <v>0</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>95</v>
       </c>
@@ -2211,11 +2101,8 @@
       <c r="F29">
         <v>0</v>
       </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>168</v>
       </c>
@@ -2234,11 +2121,8 @@
       <c r="F30">
         <v>0</v>
       </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>4</v>
       </c>
@@ -2257,11 +2141,8 @@
       <c r="F31">
         <v>0</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>192</v>
       </c>
@@ -2280,11 +2161,8 @@
       <c r="F32">
         <v>0</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>54</v>
       </c>
@@ -2303,11 +2181,8 @@
       <c r="F33">
         <v>1</v>
       </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>12</v>
       </c>
@@ -2326,11 +2201,8 @@
       <c r="F34">
         <v>0</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>205</v>
       </c>
@@ -2349,11 +2221,8 @@
       <c r="F35">
         <v>1</v>
       </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>20</v>
       </c>
@@ -2372,11 +2241,8 @@
       <c r="F36">
         <v>1</v>
       </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>238</v>
       </c>
@@ -2395,11 +2261,8 @@
       <c r="F37">
         <v>1</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>245</v>
       </c>
@@ -2418,11 +2281,8 @@
       <c r="F38">
         <v>1</v>
       </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>244</v>
       </c>
@@ -2441,11 +2301,8 @@
       <c r="F39">
         <v>1</v>
       </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>105</v>
       </c>
@@ -2464,11 +2321,8 @@
       <c r="F40">
         <v>0</v>
       </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>97</v>
       </c>
@@ -2487,11 +2341,8 @@
       <c r="F41">
         <v>0</v>
       </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>37</v>
       </c>
@@ -2510,11 +2361,8 @@
       <c r="F42">
         <v>0</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>62</v>
       </c>
@@ -2533,11 +2381,8 @@
       <c r="F43">
         <v>1</v>
       </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>26</v>
       </c>
@@ -2556,11 +2401,8 @@
       <c r="F44">
         <v>0</v>
       </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>64</v>
       </c>
@@ -2579,11 +2421,8 @@
       <c r="F45">
         <v>1</v>
       </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>150</v>
       </c>
@@ -2602,11 +2441,8 @@
       <c r="F46">
         <v>0</v>
       </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>83</v>
       </c>
@@ -2625,11 +2461,8 @@
       <c r="F47">
         <v>1</v>
       </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>69</v>
       </c>
@@ -2648,11 +2481,8 @@
       <c r="F48">
         <v>1</v>
       </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>87</v>
       </c>
@@ -2671,11 +2501,8 @@
       <c r="F49">
         <v>0</v>
       </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>42</v>
       </c>
@@ -2694,11 +2521,8 @@
       <c r="F50">
         <v>0</v>
       </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>206</v>
       </c>
@@ -2717,11 +2541,8 @@
       <c r="F51">
         <v>1</v>
       </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>46</v>
       </c>
@@ -2740,11 +2561,8 @@
       <c r="F52">
         <v>0</v>
       </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>163</v>
       </c>
@@ -2763,11 +2581,8 @@
       <c r="F53">
         <v>0</v>
       </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>113</v>
       </c>
@@ -2786,11 +2601,8 @@
       <c r="F54">
         <v>0</v>
       </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2809,11 +2621,8 @@
       <c r="F55">
         <v>0</v>
       </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>131</v>
       </c>
@@ -2832,11 +2641,8 @@
       <c r="F56">
         <v>0</v>
       </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>1</v>
       </c>
@@ -2855,11 +2661,8 @@
       <c r="F57">
         <v>1</v>
       </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>125</v>
       </c>
@@ -2878,11 +2681,8 @@
       <c r="F58">
         <v>0</v>
       </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>263</v>
       </c>
@@ -2901,11 +2701,8 @@
       <c r="F59">
         <v>0</v>
       </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>227</v>
       </c>
@@ -2924,11 +2721,8 @@
       <c r="F60">
         <v>0</v>
       </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>77</v>
       </c>
@@ -2947,11 +2741,8 @@
       <c r="F61">
         <v>0</v>
       </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>250</v>
       </c>
@@ -2964,11 +2755,8 @@
       <c r="F62">
         <v>0</v>
       </c>
-      <c r="G62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>166</v>
       </c>
@@ -2987,11 +2775,8 @@
       <c r="F63">
         <v>0</v>
       </c>
-      <c r="G63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>73</v>
       </c>
@@ -3010,11 +2795,8 @@
       <c r="F64">
         <v>1</v>
       </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>226</v>
       </c>
@@ -3027,11 +2809,8 @@
       <c r="F65">
         <v>0</v>
       </c>
-      <c r="G65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>152</v>
       </c>
@@ -3050,11 +2829,8 @@
       <c r="F66">
         <v>1</v>
       </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>16</v>
       </c>
@@ -3073,11 +2849,8 @@
       <c r="F67">
         <v>0</v>
       </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>273</v>
       </c>
@@ -3096,11 +2869,8 @@
       <c r="F68">
         <v>0</v>
       </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>276</v>
       </c>
@@ -3119,11 +2889,8 @@
       <c r="F69">
         <v>0</v>
       </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>57</v>
       </c>
@@ -3142,11 +2909,8 @@
       <c r="F70">
         <v>0</v>
       </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>133</v>
       </c>
@@ -3165,11 +2929,8 @@
       <c r="F71">
         <v>0</v>
       </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>136</v>
       </c>
@@ -3188,11 +2949,8 @@
       <c r="F72">
         <v>0</v>
       </c>
-      <c r="G72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>172</v>
       </c>
@@ -3211,11 +2969,8 @@
       <c r="F73">
         <v>1</v>
       </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>112</v>
       </c>
@@ -3234,11 +2989,8 @@
       <c r="F74">
         <v>0</v>
       </c>
-      <c r="G74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>175</v>
       </c>
@@ -3257,11 +3009,8 @@
       <c r="F75">
         <v>1</v>
       </c>
-      <c r="G75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>236</v>
       </c>
@@ -3280,11 +3029,8 @@
       <c r="F76">
         <v>0</v>
       </c>
-      <c r="G76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>217</v>
       </c>
@@ -3303,11 +3049,8 @@
       <c r="F77">
         <v>1</v>
       </c>
-      <c r="G77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>30</v>
       </c>
@@ -3326,11 +3069,8 @@
       <c r="F78">
         <v>1</v>
       </c>
-      <c r="G78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>21</v>
       </c>
@@ -3349,11 +3089,8 @@
       <c r="F79">
         <v>0</v>
       </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>256</v>
       </c>
@@ -3372,11 +3109,8 @@
       <c r="F80">
         <v>1</v>
       </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>65</v>
       </c>
@@ -3395,11 +3129,8 @@
       <c r="F81">
         <v>0</v>
       </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43</v>
       </c>
@@ -3418,11 +3149,8 @@
       <c r="F82">
         <v>0</v>
       </c>
-      <c r="G82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>210</v>
       </c>
@@ -3441,11 +3169,8 @@
       <c r="F83">
         <v>0</v>
       </c>
-      <c r="G83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>252</v>
       </c>
@@ -3464,11 +3189,8 @@
       <c r="F84">
         <v>1</v>
       </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>214</v>
       </c>
@@ -3487,11 +3209,8 @@
       <c r="F85">
         <v>0</v>
       </c>
-      <c r="G85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>123</v>
       </c>
@@ -3510,11 +3229,8 @@
       <c r="F86">
         <v>0</v>
       </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>170</v>
       </c>
@@ -3533,11 +3249,8 @@
       <c r="F87">
         <v>0</v>
       </c>
-      <c r="G87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>177</v>
       </c>
@@ -3556,11 +3269,8 @@
       <c r="F88">
         <v>1</v>
       </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>243</v>
       </c>
@@ -3579,11 +3289,8 @@
       <c r="F89">
         <v>0</v>
       </c>
-      <c r="G89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>36</v>
       </c>
@@ -3602,11 +3309,8 @@
       <c r="F90">
         <v>0</v>
       </c>
-      <c r="G90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>84</v>
       </c>
@@ -3625,11 +3329,8 @@
       <c r="F91">
         <v>0</v>
       </c>
-      <c r="G91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>98</v>
       </c>
@@ -3648,11 +3349,8 @@
       <c r="F92">
         <v>0</v>
       </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>165</v>
       </c>
@@ -3671,11 +3369,8 @@
       <c r="F93">
         <v>0</v>
       </c>
-      <c r="G93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>146</v>
       </c>
@@ -3694,11 +3389,8 @@
       <c r="F94">
         <v>0</v>
       </c>
-      <c r="G94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>45</v>
       </c>
@@ -3717,11 +3409,8 @@
       <c r="F95">
         <v>0</v>
       </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>208</v>
       </c>
@@ -3740,11 +3429,8 @@
       <c r="F96">
         <v>0</v>
       </c>
-      <c r="G96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>182</v>
       </c>
@@ -3763,11 +3449,8 @@
       <c r="F97">
         <v>0</v>
       </c>
-      <c r="G97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>66</v>
       </c>
@@ -3780,11 +3463,8 @@
       <c r="F98">
         <v>0</v>
       </c>
-      <c r="G98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>142</v>
       </c>
@@ -3803,11 +3483,8 @@
       <c r="F99">
         <v>0</v>
       </c>
-      <c r="G99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>153</v>
       </c>
@@ -3826,11 +3503,8 @@
       <c r="F100">
         <v>0</v>
       </c>
-      <c r="G100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>76</v>
       </c>
@@ -3849,12 +3523,9 @@
       <c r="F101">
         <v>0</v>
       </c>
-      <c r="G101">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{8181C947-CEED-468B-BA64-1EEB87188487}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{A67D1EDC-1AF2-4A36-9E8E-11965E7354C0}"/>

</xml_diff>